<commit_message>
corrected reported test score results
</commit_message>
<xml_diff>
--- a/test-scores.xlsx
+++ b/test-scores.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="1500" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="31300" yWindow="3460" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="22">
   <si>
     <t>Vocabulary Pre-Test Score</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>No (t=1.274, p=0.227)</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -523,11 +526,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2127135272"/>
-        <c:axId val="2127138248"/>
+        <c:axId val="2100159592"/>
+        <c:axId val="2100968376"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2127135272"/>
+        <c:axId val="2100159592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -536,7 +539,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127138248"/>
+        <c:crossAx val="2100968376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -544,7 +547,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2127138248"/>
+        <c:axId val="2100968376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -555,7 +558,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2127135272"/>
+        <c:crossAx val="2100159592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -716,13 +719,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>3.00616650188</c:v>
+                    <c:v>3.51681674245</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.84719715194</c:v>
+                    <c:v>4.56420858419</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.9052317076</c:v>
+                    <c:v>1.08074048689</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -734,13 +737,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>3.00616650188</c:v>
+                    <c:v>3.51681674245</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>3.84719715194</c:v>
+                    <c:v>4.56420858419</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.9052317076</c:v>
+                    <c:v>1.08074048689</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -770,13 +773,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.66666666667</c:v>
+                  <c:v>5.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.16666666667</c:v>
+                  <c:v>7.8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5</c:v>
+                  <c:v>2.399999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -791,11 +794,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2126161992"/>
-        <c:axId val="2126164968"/>
+        <c:axId val="2101016632"/>
+        <c:axId val="2101019608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2126161992"/>
+        <c:axId val="2101016632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -804,7 +807,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126164968"/>
+        <c:crossAx val="2101019608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -812,7 +815,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2126164968"/>
+        <c:axId val="2101019608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -823,7 +826,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2126161992"/>
+        <c:crossAx val="2101016632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1232,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AG10"/>
+  <dimension ref="A1:AG15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1399,23 +1402,23 @@
         <v>5</v>
       </c>
       <c r="L3" s="1">
-        <v>4.6666666666700003</v>
+        <v>5.4</v>
       </c>
       <c r="M3" s="1">
-        <v>7.1666666666700003</v>
+        <v>7.8</v>
       </c>
       <c r="N3">
         <f>M3-L3</f>
-        <v>2.5</v>
+        <v>2.3999999999999995</v>
       </c>
       <c r="P3" s="1">
-        <v>3.0061665018800001</v>
+        <v>3.5168167424500001</v>
       </c>
       <c r="Q3" s="1">
-        <v>3.8471971519400001</v>
+        <v>4.5642085841900002</v>
       </c>
       <c r="R3" s="1">
-        <v>0.90523170760000005</v>
+        <v>1.0807404868899999</v>
       </c>
       <c r="W3" t="s">
         <v>5</v>
@@ -1491,6 +1494,11 @@
       </c>
       <c r="Z10" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33">
+      <c r="Q15" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>